<commit_message>
update best_implementations and plot
</commit_message>
<xml_diff>
--- a/best_implementations.xlsx
+++ b/best_implementations.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/msteiner/Documents/Doktorat/efacomp_OSF/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sgrieder/GitHub/efacomp_OSF/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30EC5B4A-EA3F-894F-82AD-FC40CFF7B4B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F66A929-D6F2-A54C-82B1-79909063C62C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="38400" windowHeight="10740" xr2:uid="{F3B92D73-2713-3542-A177-744713FBD6BE}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14020" xr2:uid="{F3B92D73-2713-3542-A177-744713FBD6BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="65">
   <si>
     <t>RMSE</t>
   </si>
@@ -250,9 +250,6 @@
     <t>ID 102</t>
   </si>
   <si>
-    <t>ID 108</t>
-  </si>
-  <si>
     <t>ID 126</t>
   </si>
   <si>
@@ -262,12 +259,6 @@
     <t>ID 150</t>
   </si>
   <si>
-    <t>ID 171</t>
-  </si>
-  <si>
-    <t>ID 106</t>
-  </si>
-  <si>
     <t>ID 174</t>
   </si>
   <si>
@@ -317,13 +308,25 @@
   </si>
   <si>
     <t>ID 80</t>
+  </si>
+  <si>
+    <t>SPSS</t>
+  </si>
+  <si>
+    <t>psych_smc</t>
+  </si>
+  <si>
+    <t>psych_unity</t>
+  </si>
+  <si>
+    <t>Number of data sets used für weighting</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -350,6 +353,13 @@
       <i/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -395,7 +405,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -461,13 +471,19 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -786,8 +802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CCA8FA2-8481-CF49-AC40-D1909F0FEBF1}">
   <dimension ref="A1:AT34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AG2" sqref="AG2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -817,7 +833,7 @@
         <v>22</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F1" s="16" t="s">
         <v>31</v>
@@ -826,10 +842,10 @@
         <v>23</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J1" s="16" t="s">
         <v>32</v>
@@ -838,13 +854,13 @@
         <v>33</v>
       </c>
       <c r="L1" s="16" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="M1" s="16" t="s">
         <v>34</v>
       </c>
       <c r="N1" s="16" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="O1" s="16" t="s">
         <v>35</v>
@@ -856,7 +872,7 @@
         <v>37</v>
       </c>
       <c r="R1" s="16" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="S1" s="16" t="s">
         <v>38</v>
@@ -868,49 +884,51 @@
         <v>40</v>
       </c>
       <c r="V1" s="16" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="W1" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="X1" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="X1" s="16" t="s">
+      <c r="Y1" s="16" t="s">
         <v>42</v>
-      </c>
-      <c r="Y1" s="16" t="s">
-        <v>43</v>
       </c>
       <c r="Z1" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AA1" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB1" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC1" s="16" t="s">
         <v>44</v>
-      </c>
-      <c r="AB1" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC1" s="16" t="s">
-        <v>47</v>
       </c>
       <c r="AD1" s="16" t="s">
         <v>25</v>
       </c>
       <c r="AE1" s="16" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="AF1" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="AG1" s="32"/>
-      <c r="AH1" s="32"/>
-      <c r="AI1" s="32"/>
-      <c r="AJ1" s="32"/>
-      <c r="AK1" s="32"/>
-      <c r="AL1" s="32"/>
-      <c r="AM1" s="32"/>
-      <c r="AN1" s="32"/>
-      <c r="AO1" s="32"/>
-      <c r="AP1" s="32"/>
-      <c r="AQ1" s="32"/>
+        <v>46</v>
+      </c>
+      <c r="AG1" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="AH1" s="31"/>
+      <c r="AI1" s="31"/>
+      <c r="AJ1" s="31"/>
+      <c r="AK1" s="31"/>
+      <c r="AL1" s="31"/>
+      <c r="AM1" s="31"/>
+      <c r="AN1" s="31"/>
+      <c r="AO1" s="31"/>
+      <c r="AP1" s="31"/>
+      <c r="AQ1" s="31"/>
       <c r="AR1" s="26"/>
       <c r="AS1" s="26"/>
       <c r="AT1" s="26"/>
@@ -1417,135 +1435,135 @@
       <c r="AR6" s="6"/>
       <c r="AS6" s="6"/>
     </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:46" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B7" s="3">
-        <f>SUMPRODUCT(B3:B6,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" ref="B7:AF7" si="0">SUMPRODUCT(B3:B6,$AG3:$AG6)/SUM($AG3:$AG6)</f>
         <v>0.72454360679114949</v>
       </c>
       <c r="C7" s="6">
-        <f>SUMPRODUCT(C3:C6,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="0"/>
         <v>0.69874487816396358</v>
       </c>
       <c r="D7" s="3">
-        <f>SUMPRODUCT(D3:D6,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="0"/>
         <v>0.71966835966979503</v>
       </c>
       <c r="E7" s="3">
-        <f>SUMPRODUCT(E3:E6,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="0"/>
         <v>0.71966835966979503</v>
       </c>
       <c r="F7" s="6">
-        <f>SUMPRODUCT(F3:F6,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="0"/>
         <v>0.70362012528531803</v>
       </c>
       <c r="G7" s="3">
-        <f>SUMPRODUCT(G3:G6,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="0"/>
         <v>0.71966835966979503</v>
       </c>
       <c r="H7" s="6">
-        <f>SUMPRODUCT(H3:H6,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="0"/>
         <v>0.50947112557700236</v>
       </c>
       <c r="I7" s="6">
-        <f>SUMPRODUCT(I3:I6,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="0"/>
         <v>0.53607295809470001</v>
       </c>
       <c r="J7" s="6">
-        <f>SUMPRODUCT(J3:J6,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="0"/>
         <v>0.54369647247288033</v>
       </c>
       <c r="K7" s="6">
-        <f>SUMPRODUCT(K3:K6,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="0"/>
         <v>0.55709695490932332</v>
       </c>
       <c r="L7" s="6">
-        <f>SUMPRODUCT(L3:L6,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="0"/>
         <v>0.50947112557700236</v>
       </c>
       <c r="M7" s="6">
-        <f>SUMPRODUCT(M3:M6,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="0"/>
         <v>0.54369647247288033</v>
       </c>
       <c r="N7" s="6">
-        <f>SUMPRODUCT(N3:N6,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="0"/>
         <v>0.51927092834290955</v>
       </c>
       <c r="O7" s="6">
-        <f>SUMPRODUCT(O3:O6,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="0"/>
         <v>0.54094820521605469</v>
       </c>
       <c r="P7" s="6">
-        <f>SUMPRODUCT(P3:P6,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="0"/>
         <v>0.55837152236014198</v>
       </c>
       <c r="Q7" s="6">
-        <f>SUMPRODUCT(Q3:Q6,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="0"/>
         <v>0.56197220203067777</v>
       </c>
       <c r="R7" s="6">
-        <f>SUMPRODUCT(R3:R6,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="0"/>
         <v>0.51434637269835681</v>
       </c>
       <c r="S7" s="6">
-        <f>SUMPRODUCT(S3:S6,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="0"/>
         <v>0.55349627523878753</v>
       </c>
       <c r="T7" s="6">
-        <f>SUMPRODUCT(T3:T6,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="0"/>
         <v>0.52357688194196872</v>
       </c>
       <c r="U7" s="6">
-        <f>SUMPRODUCT(U3:U6,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="0"/>
         <v>0.53835054887562683</v>
       </c>
       <c r="V7" s="6">
-        <f>SUMPRODUCT(V3:V6,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="0"/>
         <v>0.44666757721529543</v>
       </c>
       <c r="W7" s="6">
-        <f>SUMPRODUCT(W3:W6,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="0"/>
         <v>0.52909073231259285</v>
       </c>
       <c r="X7" s="6">
-        <f>SUMPRODUCT(X3:X6,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="0"/>
         <v>0.53835054887562683</v>
       </c>
       <c r="Y7" s="6">
-        <f>SUMPRODUCT(Y3:Y6,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="0"/>
         <v>0.67160065189108609</v>
       </c>
       <c r="Z7" s="6">
-        <f>SUMPRODUCT(Z3:Z6,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="0"/>
         <v>0.6756957131679221</v>
       </c>
       <c r="AA7" s="6">
-        <f>SUMPRODUCT(AA3:AA6,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="0"/>
         <v>0.70019885456069109</v>
       </c>
       <c r="AB7" s="6">
-        <f>SUMPRODUCT(AB3:AB6,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="0"/>
         <v>0.67572400190752224</v>
       </c>
       <c r="AC7" s="6">
-        <f>SUMPRODUCT(AC3:AC6,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="0"/>
         <v>0.70432220457712735</v>
       </c>
       <c r="AD7" s="6">
-        <f>SUMPRODUCT(AD3:AD6,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="0"/>
         <v>0.69081213221166093</v>
       </c>
       <c r="AE7" s="6">
-        <f>SUMPRODUCT(AE3:AE6,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="0"/>
         <v>0.64204234514114267</v>
       </c>
       <c r="AF7" s="6">
-        <f>SUMPRODUCT(AF3:AF6,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="0"/>
         <v>0.64204234514114267</v>
       </c>
-      <c r="AG7" s="6">
+      <c r="AG7" s="35">
         <f>MAX(B7:AF7)</f>
         <v>0.72454360679114949</v>
       </c>
@@ -1562,7 +1580,7 @@
       <c r="AR7" s="6"/>
       <c r="AS7" s="6"/>
     </row>
-    <row r="8" spans="1:46" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:46" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
@@ -1597,7 +1615,7 @@
       <c r="AD8" s="5"/>
       <c r="AE8" s="5"/>
       <c r="AF8" s="5"/>
-      <c r="AG8" s="6"/>
+      <c r="AG8" s="35"/>
       <c r="AH8" s="8"/>
       <c r="AI8" s="8"/>
       <c r="AJ8" s="8"/>
@@ -1708,7 +1726,7 @@
       <c r="AF9" s="3">
         <v>1</v>
       </c>
-      <c r="AG9" s="6"/>
+      <c r="AG9" s="35"/>
       <c r="AH9" s="11"/>
       <c r="AI9" s="11"/>
       <c r="AJ9" s="11"/>
@@ -1819,7 +1837,7 @@
       <c r="AF10" s="6">
         <v>0.9</v>
       </c>
-      <c r="AG10" s="6"/>
+      <c r="AG10" s="35"/>
       <c r="AH10" s="11"/>
       <c r="AI10" s="11"/>
       <c r="AJ10" s="10"/>
@@ -1930,7 +1948,7 @@
       <c r="AF11" s="3">
         <v>1</v>
       </c>
-      <c r="AG11" s="6"/>
+      <c r="AG11" s="35"/>
       <c r="AH11" s="11"/>
       <c r="AI11" s="11"/>
       <c r="AJ11" s="11"/>
@@ -2041,7 +2059,7 @@
       <c r="AF12" s="6">
         <v>0.89</v>
       </c>
-      <c r="AG12" s="6"/>
+      <c r="AG12" s="35"/>
       <c r="AH12" s="10"/>
       <c r="AI12" s="10"/>
       <c r="AJ12" s="10"/>
@@ -2055,135 +2073,135 @@
       <c r="AR12" s="6"/>
       <c r="AS12" s="6"/>
     </row>
-    <row r="13" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:46" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B13" s="3">
-        <f>SUMPRODUCT(B9:B12,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" ref="B13:AF13" si="1">SUMPRODUCT(B9:B12,$AG3:$AG6)/SUM($AG3:$AG6)</f>
         <v>1</v>
       </c>
       <c r="C13" s="3">
-        <f>SUMPRODUCT(C9:C12,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="D13" s="3">
-        <f>SUMPRODUCT(D9:D12,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E13" s="3">
-        <f>SUMPRODUCT(E9:E12,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="F13" s="3">
-        <f>SUMPRODUCT(F9:F12,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G13" s="3">
-        <f>SUMPRODUCT(G9:G12,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H13" s="3">
-        <f>SUMPRODUCT(H9:H12,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I13" s="3">
-        <f>SUMPRODUCT(I9:I12,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J13" s="3">
-        <f>SUMPRODUCT(J9:J12,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K13" s="3">
-        <f>SUMPRODUCT(K9:K12,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L13" s="3">
-        <f>SUMPRODUCT(L9:L12,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M13" s="3">
-        <f>SUMPRODUCT(M9:M12,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="N13" s="3">
-        <f>SUMPRODUCT(N9:N12,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="O13" s="3">
-        <f>SUMPRODUCT(O9:O12,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P13" s="3">
-        <f>SUMPRODUCT(P9:P12,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="Q13" s="3">
-        <f>SUMPRODUCT(Q9:Q12,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="R13" s="3">
-        <f>SUMPRODUCT(R9:R12,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="S13" s="3">
-        <f>SUMPRODUCT(S9:S12,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="T13" s="3">
-        <f>SUMPRODUCT(T9:T12,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="U13" s="3">
-        <f>SUMPRODUCT(U9:U12,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="V13" s="3">
-        <f>SUMPRODUCT(V9:V12,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="W13" s="6">
-        <f>SUMPRODUCT(W9:W12,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="1"/>
         <v>0.97998027659072073</v>
       </c>
       <c r="X13" s="3">
-        <f>SUMPRODUCT(X9:X12,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="Y13" s="3">
-        <f>SUMPRODUCT(Y9:Y12,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="Z13" s="3">
-        <f>SUMPRODUCT(Z9:Z12,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AA13" s="3">
-        <f>SUMPRODUCT(AA9:AA12,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AB13" s="3">
-        <f>SUMPRODUCT(AB9:AB12,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AC13" s="3">
-        <f>SUMPRODUCT(AC9:AC12,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AD13" s="6">
-        <f>SUMPRODUCT(AD9:AD12,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="1"/>
         <v>0.97998027659072073</v>
       </c>
       <c r="AE13" s="3">
-        <f>SUMPRODUCT(AE9:AE12,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="1"/>
         <v>0.99787302013547119</v>
       </c>
       <c r="AF13" s="3">
-        <f>SUMPRODUCT(AF9:AF12,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="1"/>
         <v>0.99787302013547119</v>
       </c>
-      <c r="AG13" s="6">
+      <c r="AG13" s="35">
         <f>MAX(B13:AF13)</f>
         <v>1</v>
       </c>
@@ -2200,7 +2218,7 @@
       <c r="AR13" s="3"/>
       <c r="AS13" s="3"/>
     </row>
-    <row r="14" spans="1:46" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:46" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
@@ -2235,7 +2253,7 @@
       <c r="AD14" s="5"/>
       <c r="AE14" s="5"/>
       <c r="AF14" s="5"/>
-      <c r="AG14" s="6"/>
+      <c r="AG14" s="35"/>
       <c r="AH14" s="8"/>
       <c r="AI14" s="8"/>
       <c r="AJ14" s="8"/>
@@ -2346,7 +2364,7 @@
       <c r="AF15" s="6">
         <v>0.9</v>
       </c>
-      <c r="AG15" s="6"/>
+      <c r="AG15" s="35"/>
       <c r="AH15" s="10"/>
       <c r="AI15" s="10"/>
       <c r="AJ15" s="11"/>
@@ -2457,7 +2475,7 @@
       <c r="AF16" s="6">
         <v>0.9</v>
       </c>
-      <c r="AG16" s="6"/>
+      <c r="AG16" s="35"/>
       <c r="AH16" s="11"/>
       <c r="AI16" s="11"/>
       <c r="AJ16" s="10"/>
@@ -2568,7 +2586,7 @@
       <c r="AF17" s="3">
         <v>0.94</v>
       </c>
-      <c r="AG17" s="6"/>
+      <c r="AG17" s="35"/>
       <c r="AH17" s="10"/>
       <c r="AI17" s="10"/>
       <c r="AJ17" s="10"/>
@@ -2679,7 +2697,7 @@
       <c r="AF18" s="6">
         <v>0.44</v>
       </c>
-      <c r="AG18" s="6"/>
+      <c r="AG18" s="35"/>
       <c r="AH18" s="10"/>
       <c r="AI18" s="10"/>
       <c r="AJ18" s="10"/>
@@ -2693,135 +2711,135 @@
       <c r="AR18" s="6"/>
       <c r="AS18" s="6"/>
     </row>
-    <row r="19" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:46" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B19" s="6">
-        <f>SUMPRODUCT(B15:B18,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" ref="B19:AF19" si="2">SUMPRODUCT(B15:B18,$AG3:$AG6)/SUM($AG3:$AG6)</f>
         <v>0.87767314699495802</v>
       </c>
       <c r="C19" s="6">
-        <f>SUMPRODUCT(C15:C18,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="2"/>
         <v>0.87644788806733731</v>
       </c>
       <c r="D19" s="6">
-        <f>SUMPRODUCT(D15:D18,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="2"/>
         <v>0.87274859135040539</v>
       </c>
       <c r="E19" s="6">
-        <f>SUMPRODUCT(E15:E18,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="2"/>
         <v>0.88254839411631258</v>
       </c>
       <c r="F19" s="6">
-        <f>SUMPRODUCT(F15:F18,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="2"/>
         <v>0.891073629431401</v>
       </c>
       <c r="G19" s="6">
-        <f>SUMPRODUCT(G15:G18,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="2"/>
         <v>0.88254839411631258</v>
       </c>
       <c r="H19" s="6">
-        <f>SUMPRODUCT(H15:H18,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="2"/>
         <v>0.81494821447587129</v>
       </c>
       <c r="I19" s="6">
-        <f>SUMPRODUCT(I15:I18,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="2"/>
         <v>0.8323241213591559</v>
       </c>
       <c r="J19" s="6">
-        <f>SUMPRODUCT(J15:J18,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="2"/>
         <v>0.8413720270201448</v>
       </c>
       <c r="K19" s="6">
-        <f>SUMPRODUCT(K15:K18,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="2"/>
         <v>0.83237342988235419</v>
       </c>
       <c r="L19" s="6">
-        <f>SUMPRODUCT(L15:L18,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="2"/>
         <v>0.81494821447587129</v>
       </c>
       <c r="M19" s="6">
-        <f>SUMPRODUCT(M15:M18,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="2"/>
         <v>0.83644747137559217</v>
       </c>
       <c r="N19" s="6">
-        <f>SUMPRODUCT(N15:N18,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="2"/>
         <v>0.84424900572719652</v>
       </c>
       <c r="O19" s="6">
-        <f>SUMPRODUCT(O15:O18,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="2"/>
         <v>0.85674966548912668</v>
       </c>
       <c r="P19" s="6">
-        <f>SUMPRODUCT(P15:P18,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="2"/>
         <v>0.85182510984457405</v>
       </c>
       <c r="Q19" s="6">
-        <f>SUMPRODUCT(Q15:Q18,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="2"/>
         <v>0.86167422113367931</v>
       </c>
       <c r="R19" s="6">
-        <f>SUMPRODUCT(R15:R18,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="2"/>
         <v>0.84424900572719652</v>
       </c>
       <c r="S19" s="6">
-        <f>SUMPRODUCT(S15:S18,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="2"/>
         <v>0.85182510984457405</v>
       </c>
       <c r="T19" s="6">
-        <f>SUMPRODUCT(T15:T18,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="2"/>
         <v>0.86067578141277024</v>
       </c>
       <c r="U19" s="6">
-        <f>SUMPRODUCT(U15:U18,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="2"/>
         <v>0.89589956802955739</v>
       </c>
       <c r="V19" s="6">
-        <f>SUMPRODUCT(V15:V18,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="2"/>
         <v>0.70237505035025261</v>
       </c>
       <c r="W19" s="6">
-        <f>SUMPRODUCT(W15:W18,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="2"/>
         <v>0.87725492737988864</v>
       </c>
       <c r="X19" s="6">
-        <f>SUMPRODUCT(X15:X18,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="2"/>
         <v>0.91052530939362097</v>
       </c>
       <c r="Y19" s="6">
-        <f>SUMPRODUCT(Y15:Y18,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="2"/>
         <v>0.89580095098316093</v>
       </c>
       <c r="Z19" s="3">
-        <f>SUMPRODUCT(Z15:Z18,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="2"/>
         <v>0.92794862653770827</v>
       </c>
       <c r="AA19" s="6">
-        <f>SUMPRODUCT(AA15:AA18,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="2"/>
         <v>0.91052530939362097</v>
       </c>
       <c r="AB19" s="6">
-        <f>SUMPRODUCT(AB15:AB18,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="2"/>
         <v>0.90555144522587017</v>
       </c>
       <c r="AC19" s="3">
-        <f>SUMPRODUCT(AC15:AC18,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="2"/>
         <v>0.92515105075768456</v>
       </c>
       <c r="AD19" s="6">
-        <f>SUMPRODUCT(AD15:AD18,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="2"/>
         <v>0.89670660734210861</v>
       </c>
       <c r="AE19" s="6">
-        <f>SUMPRODUCT(AE15:AE18,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="2"/>
         <v>0.9137506423997741</v>
       </c>
       <c r="AF19" s="6">
-        <f>SUMPRODUCT(AF15:AF18,$AG3:$AG6)/SUM($AG3:$AG6)</f>
+        <f t="shared" si="2"/>
         <v>0.9137506423997741</v>
       </c>
-      <c r="AG19" s="6">
+      <c r="AG19" s="35">
         <f>MAX(B19:AF19)</f>
         <v>0.92794862653770827</v>
       </c>
@@ -2838,135 +2856,135 @@
       <c r="AR19" s="6"/>
       <c r="AS19" s="6"/>
     </row>
-    <row r="20" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:46" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B20" s="6">
         <f>AVERAGE(B7,B13,B19)</f>
         <v>0.86740558459536921</v>
       </c>
       <c r="C20" s="6">
-        <f t="shared" ref="C20:AS20" si="0">AVERAGE(C7,C13,C19)</f>
+        <f t="shared" ref="C20:AF20" si="3">AVERAGE(C7,C13,C19)</f>
         <v>0.85839758874376704</v>
       </c>
       <c r="D20" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.86413898367340014</v>
       </c>
       <c r="E20" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.86740558459536921</v>
       </c>
       <c r="F20" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.86489791823890627</v>
       </c>
       <c r="G20" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.86740558459536921</v>
       </c>
       <c r="H20" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.77480644668429122</v>
       </c>
       <c r="I20" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.78946569315128523</v>
       </c>
       <c r="J20" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.79502283316434175</v>
       </c>
       <c r="K20" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.79649012826389243</v>
       </c>
       <c r="L20" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.77480644668429122</v>
       </c>
       <c r="M20" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.79338131461615757</v>
       </c>
       <c r="N20" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.78783997802336858</v>
       </c>
       <c r="O20" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.79923262356839375</v>
       </c>
       <c r="P20" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.80339887740157201</v>
       </c>
       <c r="Q20" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.80788214105478573</v>
       </c>
       <c r="R20" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.78619845947518441</v>
       </c>
       <c r="S20" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.80177379502778712</v>
       </c>
       <c r="T20" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.79475088778491287</v>
       </c>
       <c r="U20" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.81141670563506141</v>
       </c>
       <c r="V20" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.7163475425218494</v>
       </c>
       <c r="W20" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.79544197876106748</v>
       </c>
       <c r="X20" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.81629195275641597</v>
       </c>
       <c r="Y20" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.85580053429141578</v>
       </c>
       <c r="Z20" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.86788144656854349</v>
       </c>
       <c r="AA20" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.87024138798477058</v>
       </c>
       <c r="AB20" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.8604251490444641</v>
       </c>
       <c r="AC20" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.87649108511160401</v>
       </c>
       <c r="AD20" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.85583300538149676</v>
       </c>
       <c r="AE20" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.8512220025587961</v>
       </c>
       <c r="AF20" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.8512220025587961</v>
       </c>
-      <c r="AG20" s="6">
+      <c r="AG20" s="35">
         <f>MAX(B20:AF20)</f>
         <v>0.87649108511160401</v>
       </c>
@@ -3148,7 +3166,7 @@
         <v>9</v>
       </c>
       <c r="V23" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="W23" s="4" t="s">
         <v>9</v>
@@ -3175,10 +3193,10 @@
         <v>9</v>
       </c>
       <c r="AE23" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="AF23" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="AG23" s="8"/>
       <c r="AH23" s="8"/>
@@ -3218,10 +3236,10 @@
         <v>28</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="J24" s="4" t="s">
         <v>28</v>
@@ -3230,16 +3248,16 @@
         <v>28</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="M24" s="4" t="s">
         <v>28</v>
       </c>
       <c r="N24" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="O24" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="P24" s="4" t="s">
         <v>28</v>
@@ -3248,13 +3266,13 @@
         <v>28</v>
       </c>
       <c r="R24" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="S24" s="4" t="s">
         <v>28</v>
       </c>
       <c r="T24" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="U24" s="4" t="s">
         <v>28</v>
@@ -3269,7 +3287,7 @@
         <v>28</v>
       </c>
       <c r="Y24" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="Z24" s="4" t="s">
         <v>28</v>
@@ -3278,7 +3296,7 @@
         <v>28</v>
       </c>
       <c r="AB24" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="AC24" s="4" t="s">
         <v>28</v>
@@ -3287,10 +3305,10 @@
         <v>28</v>
       </c>
       <c r="AE24" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="AF24" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="AG24" s="4"/>
       <c r="AH24" s="4"/>
@@ -3698,97 +3716,97 @@
         <v>5</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="N29" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="O29" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="P29" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="Q29" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="R29" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="S29" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="T29" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="U29" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="V29" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="W29" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="X29" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="Y29" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="Z29" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="AA29" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="AB29" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="AC29" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="AD29" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="AE29" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="AF29" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="AG29" s="8"/>
       <c r="AH29" s="8"/>
@@ -3909,7 +3927,7 @@
       <c r="AK30" s="21"/>
       <c r="AL30" s="21"/>
       <c r="AM30" s="21"/>
-      <c r="AN30" s="33"/>
+      <c r="AN30" s="32"/>
       <c r="AO30" s="21"/>
       <c r="AP30" s="21"/>
       <c r="AQ30" s="19"/>
@@ -3918,54 +3936,54 @@
       <c r="AT30" s="19"/>
     </row>
     <row r="31" spans="1:46" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="31" t="s">
+      <c r="A31" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="31"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="31"/>
-      <c r="H31" s="31"/>
-      <c r="I31" s="31"/>
-      <c r="J31" s="31"/>
-      <c r="K31" s="31"/>
-      <c r="L31" s="31"/>
-      <c r="M31" s="31"/>
-      <c r="N31" s="31"/>
-      <c r="O31" s="31"/>
-      <c r="P31" s="31"/>
-      <c r="Q31" s="31"/>
-      <c r="R31" s="31"/>
-      <c r="S31" s="31"/>
-      <c r="T31" s="31"/>
-      <c r="U31" s="31"/>
-      <c r="V31" s="31"/>
-      <c r="W31" s="31"/>
-      <c r="X31" s="31"/>
-      <c r="Y31" s="31"/>
-      <c r="Z31" s="31"/>
-      <c r="AA31" s="31"/>
-      <c r="AB31" s="31"/>
-      <c r="AC31" s="31"/>
-      <c r="AD31" s="31"/>
-      <c r="AE31" s="31"/>
-      <c r="AF31" s="31"/>
-      <c r="AG31" s="31"/>
-      <c r="AH31" s="31"/>
-      <c r="AI31" s="31"/>
-      <c r="AJ31" s="31"/>
-      <c r="AK31" s="31"/>
-      <c r="AL31" s="31"/>
-      <c r="AM31" s="31"/>
-      <c r="AN31" s="31"/>
-      <c r="AO31" s="31"/>
-      <c r="AP31" s="31"/>
-      <c r="AQ31" s="31"/>
-      <c r="AR31" s="31"/>
-      <c r="AS31" s="31"/>
-      <c r="AT31" s="31"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="33"/>
+      <c r="H31" s="33"/>
+      <c r="I31" s="33"/>
+      <c r="J31" s="33"/>
+      <c r="K31" s="33"/>
+      <c r="L31" s="33"/>
+      <c r="M31" s="33"/>
+      <c r="N31" s="33"/>
+      <c r="O31" s="33"/>
+      <c r="P31" s="33"/>
+      <c r="Q31" s="33"/>
+      <c r="R31" s="33"/>
+      <c r="S31" s="33"/>
+      <c r="T31" s="33"/>
+      <c r="U31" s="33"/>
+      <c r="V31" s="33"/>
+      <c r="W31" s="33"/>
+      <c r="X31" s="33"/>
+      <c r="Y31" s="33"/>
+      <c r="Z31" s="33"/>
+      <c r="AA31" s="33"/>
+      <c r="AB31" s="33"/>
+      <c r="AC31" s="33"/>
+      <c r="AD31" s="33"/>
+      <c r="AE31" s="33"/>
+      <c r="AF31" s="33"/>
+      <c r="AG31" s="33"/>
+      <c r="AH31" s="33"/>
+      <c r="AI31" s="33"/>
+      <c r="AJ31" s="33"/>
+      <c r="AK31" s="33"/>
+      <c r="AL31" s="33"/>
+      <c r="AM31" s="33"/>
+      <c r="AN31" s="33"/>
+      <c r="AO31" s="33"/>
+      <c r="AP31" s="33"/>
+      <c r="AQ31" s="33"/>
+      <c r="AR31" s="33"/>
+      <c r="AS31" s="33"/>
+      <c r="AT31" s="33"/>
     </row>
     <row r="32" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A32" s="5"/>

</xml_diff>